<commit_message>
Fix errors in column names, as per https://github.com/rfordatascience/tidytuesday/issues/396
</commit_message>
<xml_diff>
--- a/data/2021/2021-11-30/data_dictionary.xlsx
+++ b/data/2021/2021-11-30/data_dictionary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hassan.mirbahar.UNDPFJ\Documents\R Projects\cricket_modelling\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jacqu\Documents\GitHub\tidytuesday\data\2021\2021-11-30\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9EB76BBB-4DC4-4FCC-9E54-97497CE4F135}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E287786-2DA9-4B8D-9E94-F591D5048099}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BE0B6879-8260-4AF7-899C-9AC07686E37F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BE0B6879-8260-4AF7-899C-9AC07686E37F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="53">
   <si>
     <t>match_id</t>
   </si>
@@ -54,9 +54,6 @@
     <t>wickets_team2</t>
   </si>
   <si>
-    <t>wickets_team</t>
-  </si>
-  <si>
     <t>team1_away_or_home</t>
   </si>
   <si>
@@ -126,9 +123,6 @@
     <t>Team one score</t>
   </si>
   <si>
-    <t>team one score</t>
-  </si>
-  <si>
     <t xml:space="preserve">wickets fallen for team one; if 10 it means all out. </t>
   </si>
   <si>
@@ -190,6 +184,15 @@
   </si>
   <si>
     <t>Number</t>
+  </si>
+  <si>
+    <t>wickets_team1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wickets fallen for team two; if 10 it means all out. </t>
+  </si>
+  <si>
+    <t>Team two score</t>
   </si>
 </sst>
 </file>
@@ -544,7 +547,7 @@
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -556,13 +559,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" t="s">
         <v>24</v>
-      </c>
-      <c r="B1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -570,10 +573,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -581,10 +584,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -592,10 +595,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -603,10 +606,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -614,219 +617,219 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C6" t="s">
-        <v>30</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="B7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" t="s">
         <v>51</v>
-      </c>
-      <c r="C8" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C12" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C13" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C14" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C15" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C16" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C18" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C19" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B20" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C20" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B21" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C21" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B22" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C22" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B23" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C23" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B24" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C24" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B25" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C25" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>